<commit_message>
Test cases with the Bioblank and Diagnosis filters
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Biobank-CCOGC.xlsx
+++ b/InputFiles/TC01_Canine_Biobank-CCOGC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836A21DE-67CA-4553-A568-C410D974A4C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB209F1C-1F95-4266-8A4E-14D6C7EF3EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -68,30 +68,33 @@
   <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis), (r:registration)--&gt;(c)
 WHERE r.registration_origin = "CCOGC"
+MATCH (c)&lt;--(diag:diagnosis)
 OPTIONAL MATCH (samp:sample)--&gt;(c)
 OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co
-RETURN  coalesce(c.case_id, '') AS `Case ID` ,
-        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
-        coalesce(s.clinical_study_type, '') AS  `Study Type`,
-        coalesce(demo.breed, '') AS Breed ,
-        coalesce(diag.disease_term, '') AS Diagnosis ,
-        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
-        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
-        coalesce(demo.sex, '') AS Sex ,
-        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-        coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`,
-		coalesce(co.cohort_description, '') AS `Cohort`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis), (r:registration)--&gt;(c)
-WHERE r.registration_origin = "CCOGC" 
- WITH DISTINCT samp AS samp, c, demo, diag
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  
+       coalesce(c.case_id, '') AS `Case ID`,
+       coalesce(s.clinical_study_designation, '') AS `Study Code`,
+       coalesce(s.clinical_study_type, '') AS  `Study Type`,
+       coalesce(demo.breed, '') AS Breed ,
+       coalesce(diag.disease_term, '') AS Diagnosis ,
+       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+       coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`
+Order by c.case_id LIMIT 100</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis), (r:registration)--&gt;(c) 
+WHERE r.registration_origin = "CCOGC"
+WITH DISTINCT samp AS samp, c, demo, diag
 RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
         coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(demo.breed,'') AS Breed,
+        coalesce(diag.disease_term,'') AS Diagnosis, 
         coalesce(samp.sample_site, '') AS `Sample Site`,
         coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
         coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
@@ -99,51 +102,89 @@
         coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
         coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
         coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
+Order by samp.sample_id LIMIT 100</t>
   </si>
   <si>
     <t>MATCH (f:file)--&gt;(parent)
 WITH DISTINCT f, parent
+MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
 MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
- MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
 MATCH (r:registration)--&gt;(c)
-WHERE r.registration_origin = "CCOGC" 
- WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
-        coalesce(f.file_type, '') AS `File Type`, 
+WHERE r.registration_origin = "CCOGC"
+OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
+WITH
+        f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value, 
+        10^precision AS factor,
+        units[i] as unit
+WITH    
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN 
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_format, '') AS `Format`,
+        coalesce(f.file_type, '') AS `File Type`,
+       CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
         coalesce(labels(parent)[0], '') AS `Association`,
         coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `File Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MATCH (f:file)--&gt;(s:study)
-MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis), (r:registration)--&gt;(c)
-WHERE r.registration_origin = "CCOGC" 
-WITH DISTINCT f, s
-RETURN 
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(demo.breed,'') AS Breed ,
+        coalesce(diag.disease_term,'') AS Diagnosis
+Order By f.file_name LIMIT 100</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(s:study)
+MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
+MATCH (r:registration)--&gt;(c)
+WHERE r.registration_origin = "CCOGC"
+WITH DISTINCT f,  s, c, demo, diag
+WITH
+        f, c, demo, diag, s,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH    
+        f, c, demo, diag, s,
+        f.file_size /(1024^i) AS value, 10^precision AS factor,
+        units[i] as unit
+        WITH    
+        f,  c, demo, diag, s, unit,
+        round(factor * value)/factor AS size
+RETURN DISTINCT
   coalesce(f.file_name, '') AS `File Name`,
   coalesce(f.file_type, '') AS `File Type`,
   coalesce("study", '') AS `Association`,
   coalesce(f.file_description, '') AS `Description`,
-  coalesce(f.file_format, '') AS `File Format`,
-  coalesce(f.file_size, '') AS `Size`,
-  coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>MATCH (p:program)&lt;--(s:study)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis), (c)&lt;--(r:registration)
-	WHERE r.registration_origin = "CCOGC"
+  coalesce(f.file_format, '') AS  Format,
+  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+  coalesce(s.clinical_study_designation,'') AS `Study Code`
+  order by 'File Name' asc
+  limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
 OPTIONAL MATCH (f:file)-[*]-&gt;(c)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-RETURN
-	count(DISTINCT(f)) as number_of_files , 
-    count(DISTINCT(samp)) as number_of_sample , 
-    count(DISTINCT(c.case_id)) as number_of_cases , 
-    count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+MATCH (r:registration)--&gt;(c)
+WHERE r.registration_origin = "CCOGC"
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
   </si>
 </sst>
 </file>
@@ -519,7 +560,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,7 +588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -564,7 +605,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -581,7 +622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -598,7 +639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>

</xml_diff>